<commit_message>
Handle quotes in hyperlink sheet names in hyperlink adresses vaadin/spreadsheet#18568
If sheet name contains only numbers its enclosing single quotes are removed
Same for sheet names including spaces
Also solves (SHEET-98)
Change-Id: I0ada3e6ff949dd77dc9e852d446a08a1bccf5ccb
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/hyper_links.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/hyper_links.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="2015" sheetId="3" r:id="rId3"/>
+    <sheet name="two words" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>This link goes to google</t>
   </si>
@@ -41,6 +43,12 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Link to B3 on sheet '2015'</t>
+  </si>
+  <si>
+    <t>Link to C3 on sheet 'two words'</t>
   </si>
 </sst>
 </file>
@@ -426,7 +434,7 @@
   <dimension ref="B5:AO164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -449,7 +457,12 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="C9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="2:4">
       <c r="D11" s="1" t="s">
@@ -509,6 +522,8 @@
     <hyperlink ref="D11" r:id="rId3" display="http://google.fi"/>
     <hyperlink ref="AO164" r:id="rId4"/>
     <hyperlink ref="C18" r:id="rId5" tooltip="tooltip text is not address"/>
+    <hyperlink ref="B9" location="'2015'!B3" display="Link to B3 on sheet '2015'"/>
+    <hyperlink ref="C9" location="'two words'!C3" display="Link to C3 on sheet 'two words'"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -549,4 +564,54 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="3:3">
+      <c r="C3">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>